<commit_message>
commit after first publish
</commit_message>
<xml_diff>
--- a/RetailAppWPF/Assets/catalog-square.xlsx
+++ b/RetailAppWPF/Assets/catalog-square.xlsx
@@ -1451,7 +1451,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -4182,7 +4182,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -4244,7 +4244,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -4554,7 +4554,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -4740,7 +4740,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -4864,7 +4864,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -5112,7 +5112,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -5298,7 +5298,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -5360,7 +5360,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -5484,7 +5484,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -5980,7 +5980,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -6166,7 +6166,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -6290,7 +6290,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -6353,7 +6353,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -6415,7 +6415,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -6539,7 +6539,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -6725,7 +6725,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -6787,7 +6787,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -7221,7 +7221,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -7469,7 +7469,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
@@ -7593,7 +7593,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -7779,7 +7779,7 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
@@ -8089,7 +8089,7 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
@@ -8151,7 +8151,7 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
@@ -8213,7 +8213,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
@@ -8275,7 +8275,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
@@ -8647,7 +8647,7 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
@@ -8709,7 +8709,7 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
@@ -8957,7 +8957,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -9453,7 +9453,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -9825,7 +9825,7 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
@@ -9887,7 +9887,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
@@ -10011,7 +10011,7 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
@@ -10073,7 +10073,7 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
@@ -10472,12 +10472,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>NSTBKQS5543JQGN57R7YMS5D</t>
+          <t>ZJPNULDRSO3I3IGTJOZQSZIG</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Vegetarian Miracle</t>
+          <t>Urban Daily Kit</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -10487,27 +10487,27 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Natural Tech</t>
+          <t>Skin Regimen</t>
         </is>
       </c>
       <c r="E163" t="inlineStr" s="2">
         <is>
-          <t>D/VEGM250</t>
+          <t>DS-KIT</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>Regular 250ml</t>
+          <t>Regular</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>37.00</t>
+          <t>99.00</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>4</t>
+          <t/>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -10517,12 +10517,12 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t/>
         </is>
       </c>
       <c r="K163" t="inlineStr">
         <is>
-          <t>2</t>
+          <t/>
         </is>
       </c>
       <c r="L163" t="inlineStr">
@@ -10534,7 +10534,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>H5J6ENQ4ZEHHHRM5PZSWZ3EA</t>
+          <t>NSTBKQS5543JQGN57R7YMS5D</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -10554,22 +10554,22 @@
       </c>
       <c r="E164" t="inlineStr" s="2">
         <is>
-          <t>D/VEGM1000</t>
+          <t>D/VEGM250</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>1000ml</t>
+          <t>Regular 250ml</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>91.00</t>
+          <t>37.00</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -10579,12 +10579,12 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
         <is>
-          <t/>
+          <t>2</t>
         </is>
       </c>
       <c r="L164" t="inlineStr">
@@ -10596,42 +10596,42 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>7IYTAYWOE3YUGHXVHNTRWGUH</t>
+          <t>H5J6ENQ4ZEHHHRM5PZSWZ3EA</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>VOLU Hair Mist 250ml</t>
+          <t>Vegetarian Miracle</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>For hair in need of a volume boost. VOLU Hair Mist creates a base for fuller-looking and bouncy hair, while increasing softness and shine.</t>
+          <t/>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Essentials</t>
+          <t>Natural Tech</t>
         </is>
       </c>
       <c r="E165" t="inlineStr" s="2">
         <is>
-          <t>D/VM2</t>
+          <t>D/VEGM1000</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t/>
+          <t>1000ml</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>39.00</t>
+          <t>91.00</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
@@ -10641,12 +10641,12 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
         <is>
-          <t>2</t>
+          <t/>
         </is>
       </c>
       <c r="L165" t="inlineStr">
@@ -10658,17 +10658,17 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>6BTZHMIY2S235BKKG2H5KAOC</t>
+          <t>7IYTAYWOE3YUGHXVHNTRWGUH</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>VOLU Shampoo</t>
+          <t>VOLU Hair Mist 250ml</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t/>
+          <t>For hair in need of a volume boost. VOLU Hair Mist creates a base for fuller-looking and bouncy hair, while increasing softness and shine.</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -10678,22 +10678,22 @@
       </c>
       <c r="E166" t="inlineStr" s="2">
         <is>
-          <t>D/VS2</t>
+          <t>D/VM2</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Regular 250ml</t>
+          <t/>
         </is>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>30.00</t>
+          <t>39.00</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -10720,7 +10720,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>HENDKHWKZNRUZEU5AOZ4NIJ7</t>
+          <t>6BTZHMIY2S235BKKG2H5KAOC</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -10740,22 +10740,22 @@
       </c>
       <c r="E167" t="inlineStr" s="2">
         <is>
-          <t>D/VS1</t>
+          <t>D/VS2</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Large 1000ml</t>
+          <t>Regular 250ml</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>62.00</t>
+          <t>30.00</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
@@ -10765,12 +10765,12 @@
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t/>
+          <t>Y</t>
         </is>
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t/>
+          <t>2</t>
         </is>
       </c>
       <c r="L167" t="inlineStr">
@@ -10782,12 +10782,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>5BW4VZ3WXPTSZ4QCHJU7TQ4G</t>
+          <t>HENDKHWKZNRUZEU5AOZ4NIJ7</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Volume Boosting Mousse</t>
+          <t>VOLU Shampoo</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -10797,27 +10797,27 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Styling</t>
+          <t>Essentials</t>
         </is>
       </c>
       <c r="E168" t="inlineStr" s="2">
         <is>
-          <t>D/MIVBM250</t>
+          <t>D/VS1</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t/>
+          <t>Large 1000ml</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>30.00</t>
+          <t>62.00</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
@@ -10827,12 +10827,12 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t/>
         </is>
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>2</t>
+          <t/>
         </is>
       </c>
       <c r="L168" t="inlineStr">
@@ -10844,12 +10844,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2XSE2KIMDCNIA2YYEU2W2PUE</t>
+          <t>5BW4VZ3WXPTSZ4QCHJU7TQ4G</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Wake Up Hair Mask</t>
+          <t>Volume Boosting Mousse</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -10859,27 +10859,27 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Circle Chronicles</t>
+          <t>Styling</t>
         </is>
       </c>
       <c r="E169" t="inlineStr" s="2">
         <is>
-          <t>D-10090010</t>
+          <t>D/MIVBM250</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>Regular</t>
+          <t/>
         </is>
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>10.00</t>
+          <t>30.00</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
@@ -10894,7 +10894,7 @@
       </c>
       <c r="K169" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L169" t="inlineStr">
@@ -10906,12 +10906,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>NJK5CKFW2CDCEMF34D76TVWW</t>
+          <t>2XSE2KIMDCNIA2YYEU2W2PUE</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Well-Being Conditioner</t>
+          <t>Wake Up Hair Mask</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -10921,27 +10921,27 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Natural Tech</t>
+          <t>Circle Chronicles</t>
         </is>
       </c>
       <c r="E170" t="inlineStr" s="2">
         <is>
-          <t>D/WBCON150</t>
+          <t>D-10090010</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>Regular 150ml</t>
+          <t>Regular</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>31.00</t>
+          <t>10.00</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>18</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -10956,7 +10956,7 @@
       </c>
       <c r="K170" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="L170" t="inlineStr">
@@ -10968,12 +10968,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Q5Z6ZJUVBILQ6T2HYNE7B24Z</t>
+          <t>NJK5CKFW2CDCEMF34D76TVWW</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Well-Being De Stress Lotion</t>
+          <t>Well-Being Conditioner</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -10988,22 +10988,22 @@
       </c>
       <c r="E171" t="inlineStr" s="2">
         <is>
-          <t>D/WBLOT250</t>
+          <t>D/WBCON150</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Regular 250ml</t>
+          <t>Regular 150ml</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>28.00</t>
+          <t>31.00</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
@@ -11018,7 +11018,7 @@
       </c>
       <c r="K171" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L171" t="inlineStr">
@@ -11030,12 +11030,12 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>LIRW77WLXB275CVJMWHYPP2T</t>
+          <t>Q5Z6ZJUVBILQ6T2HYNE7B24Z</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Well-Being Shampoo</t>
+          <t>Well-Being De Stress Lotion</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -11050,7 +11050,7 @@
       </c>
       <c r="E172" t="inlineStr" s="2">
         <is>
-          <t>D/WBSH250</t>
+          <t>D/WBLOT250</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -11060,12 +11060,12 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>31.00</t>
+          <t>28.00</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
@@ -11080,7 +11080,7 @@
       </c>
       <c r="K172" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L172" t="inlineStr">
@@ -11092,60 +11092,122 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
+          <t>LIRW77WLXB275CVJMWHYPP2T</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Well-Being Shampoo</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Natural Tech</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr" s="2">
+        <is>
+          <t>D/WBSH250</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Regular 250ml</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>31.00</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
           <t>RUEOTDGJPM6AWQJC3OTCUNNM</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
+      <c r="B174" t="inlineStr">
         <is>
           <t>Well-Being Shampoo</t>
         </is>
       </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
+      <c r="C174" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
         <is>
           <t>Natural Tech</t>
         </is>
       </c>
-      <c r="E173" t="inlineStr" s="2">
+      <c r="E174" t="inlineStr" s="2">
         <is>
           <t>D/WBSH1000</t>
         </is>
       </c>
-      <c r="F173" t="inlineStr">
+      <c r="F174" t="inlineStr">
         <is>
           <t>1000ml</t>
         </is>
       </c>
-      <c r="G173" t="inlineStr">
+      <c r="G174" t="inlineStr">
         <is>
           <t>65.00</t>
         </is>
       </c>
-      <c r="H173" t="inlineStr">
+      <c r="H174" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="I173" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J173" t="inlineStr">
+      <c r="I174" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="K173" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L173" t="inlineStr">
+      <c r="K174" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
         <is>
           <t>Y</t>
         </is>

</xml_diff>